<commit_message>
Gas: Engie XLSX parser should halt on first blank
</commit_message>
<xml_diff>
--- a/test/gas/bills.engie.xlsx
+++ b/test/gas/bills.engie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="invoice_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t xml:space="preserve">Invoice Number</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">The Apothecary, Branching Tree, The Common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoice data provided by X.</t>
   </si>
   <si>
     <t xml:space="preserve">Read</t>
@@ -204,45 +207,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B10:AH11"/>
+  <dimension ref="B10:AH13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AH12" activeCellId="0" sqref="AH12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.2753036437247"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5668016194332"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="1.92712550607287"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.92712550607287"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="1.82186234817814"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85425101214575"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.82186234817814"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="1.92712550607287"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="1.82186234817814"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.0688259109312"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.17813765182186"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.2834008097166"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.57085020242915"/>
@@ -409,6 +412,11 @@
       </c>
       <c r="AH11" s="0" t="n">
         <v>87.01</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -429,16 +437,16 @@
   </sheetPr>
   <dimension ref="B10:M11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.2753036437247"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.5991902834008"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6"/>
@@ -468,22 +476,22 @@
         <v>5</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="K10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="L10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>7</v>
@@ -512,7 +520,7 @@
         <v>42461</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>1488</v>
@@ -521,7 +529,7 @@
         <v>42466</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>94</v>

</xml_diff>

<commit_message>
Gas: Engie XLSX can't import consumption tab
</commit_message>
<xml_diff>
--- a/test/gas/bills.engie.xlsx
+++ b/test/gas/bills.engie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="invoice_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t xml:space="preserve">Invoice Number</t>
   </si>
@@ -209,43 +209,43 @@
   </sheetPr>
   <dimension ref="B10:AH13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.919028340081"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.6761133603239"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.3522267206478"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="1.82186234817814"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.85425101214575"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.82186234817814"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="1.71255060728745"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.96356275303644"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.71255060728745"/>
     <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="1.82186234817814"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="1.71255060728745"/>
     <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.42914979757085"/>
     <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.1781376518219"/>
     <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.96356275303644"/>
     <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.2834008097166"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.39271255060729"/>
     <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.49797570850202"/>
     <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.57085020242915"/>
@@ -435,18 +435,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B10:M11"/>
+  <dimension ref="B10:M13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.5991902834008"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.919028340081"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6"/>
@@ -535,6 +535,11 @@
         <v>94</v>
       </c>
     </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
gas: Bill reference the same within a batch
</commit_message>
<xml_diff>
--- a/test/gas/bills.engie.xlsx
+++ b/test/gas/bills.engie.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="invoice_data" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t xml:space="preserve">Invoice Number</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t xml:space="preserve">The Apothecary, Branching Tree, The Common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portray Castle, Ayreshire, Scotland</t>
   </si>
   <si>
     <t xml:space="preserve">Invoice data provided by X.</t>
@@ -181,13 +184,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -207,48 +214,48 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B10:AH13"/>
+  <dimension ref="B10:AH14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AH13" activeCellId="0" sqref="AH13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="43.919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0323886639676"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.6761133603239"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.03643724696356"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="1.71255060728745"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.96356275303644"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="1.71255060728745"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="1.71255060728745"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="8.03238866396761"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="6.96356275303644"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.49797570850202"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.6113360323887"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="11.17004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.18218623481781"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.17004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.9473684210526"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.9311740890688"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.8097165991903"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.20647773279352"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.1336032388664"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.30364372469636"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.1336032388664"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="6.20647773279352"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6113360323887"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="5.10526315789474"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="2.34817813765182"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.51417004048583"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="2.34817813765182"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="9.2914979757085"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="2.34817813765182"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="6.75708502024292"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="7.86234817813765"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="9.84615384615385"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="7.30364372469636"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="7.97165991902834"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="7.30364372469636"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="7.09311740890688"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,9 +421,101 @@
         <v>87.01</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>8549991</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>42496</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>42461</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>42490</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>87614362</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>89.4</v>
+      </c>
+      <c r="N12" s="0" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>0.0534</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>87.1</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>32.04</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="0" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="AA12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="0" t="n">
+        <v>9.32</v>
+      </c>
+      <c r="AE12" s="0" t="n">
+        <v>98.5</v>
+      </c>
+      <c r="AF12" s="0" t="n">
+        <v>66.1</v>
+      </c>
+      <c r="AG12" s="0" t="n">
+        <v>4.83</v>
+      </c>
+      <c r="AH12" s="0" t="n">
+        <v>302.33</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -435,18 +534,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B10:M13"/>
+  <dimension ref="B10:M14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="45.6315789473684"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.35627530364373"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="6"/>
@@ -476,22 +575,22 @@
         <v>5</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="K10" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>25</v>
-      </c>
       <c r="L10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M10" s="0" t="s">
         <v>7</v>
@@ -520,7 +619,7 @@
         <v>42461</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>1488</v>
@@ -529,15 +628,53 @@
         <v>42466</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M11" s="0" t="n">
         <v>94</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>8549991</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>42496</v>
+      </c>
+      <c r="D12" s="0" t="s">
         <v>23</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>87614362</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>42470</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <v>42478</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>